<commit_message>
add toJSONObject() in the Sample Experiment, create JSON file in the Package Compiler, and had to re-add the excel file because it wasnt importing data.
</commit_message>
<xml_diff>
--- a/out/production/CSSE374-JUMP/JUMPS-data-example.xlsx
+++ b/out/production/CSSE374-JUMP/JUMPS-data-example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kimtracy/Dropbox/Rose-Hulman/CSSE374/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C5BC44-0F43-4944-8818-0FE5641619DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A6227F-DEDF-E842-B764-09E5CAFC991D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80720" yWindow="-280" windowWidth="27640" windowHeight="16120" xr2:uid="{DBE89B78-AC7B-084C-9A8E-61D867A96616}"/>
+    <workbookView xWindow="80920" yWindow="-400" windowWidth="27640" windowHeight="16120" xr2:uid="{DBE89B78-AC7B-084C-9A8E-61D867A96616}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <sheet name="Experiment" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="182">
   <si>
     <t>Experiment Name</t>
   </si>
@@ -589,6 +588,12 @@
 - Reagent: They will need to not only specify where, but the list of reagents.  The JUMPS system should produce the command stream needed (add, mix, measure).
 - Complex: Here, the scientists also need to specify an explicit set of commands to be done by the JIU.
 </t>
+  </si>
+  <si>
+    <t>C20</t>
+  </si>
+  <si>
+    <t>updated</t>
   </si>
 </sst>
 </file>
@@ -629,18 +634,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -955,16 +961,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94EACDF5-0CF9-6D4B-9F34-795C94F1898A}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>178</v>
       </c>
       <c r="B1" s="2"/>
@@ -977,193 +983,201 @@
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>181</v>
+      </c>
+      <c r="B19" s="5">
+        <v>44313</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1179,7 +1193,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1357,7 +1371,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B17" t="s">
         <v>144</v>
@@ -1368,7 +1382,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B18" t="s">
         <v>147</v>
@@ -1379,7 +1393,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B19" t="s">
         <v>149</v>
@@ -1390,7 +1404,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>150</v>
+        <v>175</v>
       </c>
       <c r="B20" t="s">
         <v>151</v>
@@ -1398,7 +1412,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="B21" t="s">
         <v>174</v>

</xml_diff>